<commit_message>
Finalised reports and summary sheets
</commit_message>
<xml_diff>
--- a/Architecture and parameter search/results/separate/tf/tfSummary.xlsx
+++ b/Architecture and parameter search/results/separate/tf/tfSummary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\research\deepBrain\Architecture and parameter search\results\separate\tf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F5042D-9B71-44BA-9F47-A2A8C85BFC9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60E8515-68F4-4B27-9DDC-6E77EBA83265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="14" activeTab="19" xr2:uid="{70AAAB36-7ED8-4106-9A4F-E38CF3BF8A80}"/>
   </bookViews>
@@ -18364,7 +18364,7 @@
                   <c:v>0.96299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.9999999999999993E-3</c:v>
+                  <c:v>0.99099999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.91900000000000004</c:v>
@@ -18459,7 +18459,7 @@
                   <c:v>0.95499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5999999999999999E-2</c:v>
+                  <c:v>0.97399999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.85799999999999998</c:v>
@@ -18554,7 +18554,7 @@
                   <c:v>0.94099999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9000000000000001E-2</c:v>
+                  <c:v>0.97099999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.79300000000000004</c:v>
@@ -19082,13 +19082,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8.9999999999999993E-3</c:v>
+                  <c:v>0.99099999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5999999999999999E-2</c:v>
+                  <c:v>0.97399999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9000000000000001E-2</c:v>
+                  <c:v>0.97099999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19622,7 +19622,7 @@
                   <c:v>0.96499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>0.98499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.73899999999999999</c:v>
@@ -19717,7 +19717,7 @@
                   <c:v>0.95499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5999999999999999E-2</c:v>
+                  <c:v>0.97399999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.85799999999999998</c:v>
@@ -19812,7 +19812,7 @@
                   <c:v>0.94099999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9000000000000001E-2</c:v>
+                  <c:v>0.97099999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.79300000000000004</c:v>
@@ -20904,13 +20904,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>0.98499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5999999999999999E-2</c:v>
+                  <c:v>0.97399999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9000000000000001E-2</c:v>
+                  <c:v>0.97099999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -55613,7 +55613,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="I5" sqref="I5:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55657,7 +55657,7 @@
         <v>0.96499999999999997</v>
       </c>
       <c r="D5">
-        <v>1.4999999999999999E-2</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="E5">
         <v>0.73899999999999999</v>
@@ -55680,7 +55680,7 @@
         <v>0.95499999999999996</v>
       </c>
       <c r="D6">
-        <v>2.5999999999999999E-2</v>
+        <v>0.97399999999999998</v>
       </c>
       <c r="E6">
         <v>0.85799999999999998</v>
@@ -55703,7 +55703,7 @@
         <v>0.94099999999999995</v>
       </c>
       <c r="D7">
-        <v>2.9000000000000001E-2</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="E7">
         <v>0.79300000000000004</v>
@@ -55731,7 +55731,7 @@
         <v>0.96299999999999997</v>
       </c>
       <c r="D17">
-        <v>8.9999999999999993E-3</v>
+        <v>0.99099999999999999</v>
       </c>
       <c r="E17">
         <v>0.91900000000000004</v>
@@ -55754,7 +55754,7 @@
         <v>0.95499999999999996</v>
       </c>
       <c r="D18">
-        <v>2.5999999999999999E-2</v>
+        <v>0.97399999999999998</v>
       </c>
       <c r="E18">
         <v>0.85799999999999998</v>
@@ -55777,7 +55777,7 @@
         <v>0.94099999999999995</v>
       </c>
       <c r="D19">
-        <v>2.9000000000000001E-2</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="E19">
         <v>0.79300000000000004</v>

</xml_diff>